<commit_message>
BOM Update and Schematic Update
</commit_message>
<xml_diff>
--- a/BOMs/Bill of Materials.xlsx
+++ b/BOMs/Bill of Materials.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="132">
   <si>
     <t>Last modified: 2025-03-16</t>
   </si>
@@ -24,7 +24,7 @@
     <t>PCB version: 1</t>
   </si>
   <si>
-    <t>BOM revision: 6</t>
+    <t>BOM revision: 7</t>
   </si>
   <si>
     <t>P/NP</t>
@@ -99,6 +99,261 @@
     <t>72" (6 ft) 0.125" Copper Round Bar 110-H04</t>
   </si>
   <si>
+    <t>TE Connectivity Linx</t>
+  </si>
+  <si>
+    <t>CONN003-W</t>
+  </si>
+  <si>
+    <t>N Connector</t>
+  </si>
+  <si>
+    <t>DigiKey</t>
+  </si>
+  <si>
+    <t>343-CONN003-W-ND</t>
+  </si>
+  <si>
+    <t>U3, U4</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Skyworks Solutions Inc.</t>
+  </si>
+  <si>
+    <t>SKY13588-460LF</t>
+  </si>
+  <si>
+    <t>RF Switch IC WLAN SP3T 6 GHz 50Ohm 12-QFN (2x2)</t>
+  </si>
+  <si>
+    <t>863-1817-1-ND</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>SN74AVC2T244DQER</t>
+  </si>
+  <si>
+    <t>Voltage Level Translator Unidirectional 1 Circuit 2 Channel 380Mbps 8-X2SON (1.4x1)</t>
+  </si>
+  <si>
+    <t>296-29673-1-ND</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>MIC5365-1.8YC5-TR</t>
+  </si>
+  <si>
+    <t>Linear Voltage Regulator IC Positive Fixed 1 Output 150mA SC-70-5</t>
+  </si>
+  <si>
+    <t>576-3181-1-ND</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>MIC5365-3.3YC5-TR</t>
+  </si>
+  <si>
+    <t>576-3193-1-ND</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>4 Position Wire to Board Terminal Block Horizontal with Board 0.200" (5.08mm) Through Hole</t>
+  </si>
+  <si>
+    <t>277-1249-ND</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>GRM21BR61C106KE15K</t>
+  </si>
+  <si>
+    <t>10uF bypass caps</t>
+  </si>
+  <si>
+    <t>490-6473-1-ND</t>
+  </si>
+  <si>
+    <t>C5, C7</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL21A475KAQNNNE</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 25V X5R 0805</t>
+  </si>
+  <si>
+    <t>1276-1244-1-ND</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>SMBJ5.0A-13-F</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>TVS DIODE 5VWM 9.2VC SMB</t>
+  </si>
+  <si>
+    <t>SMBJ5.0A-FDICT-ND</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>C0805C561J5GACTU</t>
+  </si>
+  <si>
+    <t>560 pF ±5% 50V Ceramic Capacitor C0G, NP0 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>399-C0805C561J5GACTUCT-ND</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>DMP2008UFG-7</t>
+  </si>
+  <si>
+    <t>MOSFET P-CH 20V 14A PWRDI3333</t>
+  </si>
+  <si>
+    <t>DMP2008UFG-7DICT-ND</t>
+  </si>
+  <si>
+    <t>U13</t>
+  </si>
+  <si>
+    <t>MIC23050-SYML-TR</t>
+  </si>
+  <si>
+    <t>Buck Switching Regulator IC Positive Fixed 3.3V 1 Output 600mA 8-VFDFN Exposed Pad, 8-MLF®</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>576-3351-1-ND</t>
+  </si>
+  <si>
+    <t>J7, J8</t>
+  </si>
+  <si>
+    <t>Assmann WSW Components</t>
+  </si>
+  <si>
+    <t>AU-Y1005-2</t>
+  </si>
+  <si>
+    <t>USB-A (USB TYPE-A) USB 2.0 Receptacle Connector 4 Position Through Hole, Right Angle</t>
+  </si>
+  <si>
+    <t>AE11191-ND</t>
+  </si>
+  <si>
+    <t>J1-J4</t>
+  </si>
+  <si>
+    <t>2 Position Wire to Board Terminal Block Horizontal with Board 0.200" (5.08mm) Through Hole</t>
+  </si>
+  <si>
+    <t>277-1247-ND</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ104V</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P100KACT-ND</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>Littelfuse Inc.</t>
+  </si>
+  <si>
+    <t>RGEF300K-2</t>
+  </si>
+  <si>
+    <t>PTC RESET FUSE 16V 3A RADIAL</t>
+  </si>
+  <si>
+    <t>RGEF300K-2HFCT-ND</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>Bel Fuse Inc.</t>
+  </si>
+  <si>
+    <t>0ZCK0020FF2G</t>
+  </si>
+  <si>
+    <t>PTC RESET FUSE 9V 200MA 0805</t>
+  </si>
+  <si>
+    <t>5923-0ZCK0020FF2GCT-ND</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+  </si>
+  <si>
+    <t>MLZ2012M1R0HT000</t>
+  </si>
+  <si>
+    <t>FIXED IND 1UH 800MA 100 MOHM SMD</t>
+  </si>
+  <si>
+    <t>445-8657-1-ND</t>
+  </si>
+  <si>
     <t>TOTAL:</t>
   </si>
   <si>
@@ -114,6 +369,9 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>Power Board</t>
+  </si>
+  <si>
     <t>v1.0</t>
   </si>
   <si>
@@ -148,6 +406,12 @@
   </si>
   <si>
     <t>Fixed mismatched versions</t>
+  </si>
+  <si>
+    <t>V7.0</t>
+  </si>
+  <si>
+    <t>Ordered Power Management Board, N Connectors, and Filter Board IC's</t>
   </si>
 </sst>
 </file>
@@ -158,7 +422,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -197,8 +461,32 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,8 +499,14 @@
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border/>
     <border>
       <left/>
@@ -220,11 +514,55 @@
       <top/>
       <bottom/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0000FF"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF0000FF"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF0000FF"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF0000FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF0000FF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0000FF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0000FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF0000FF"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -254,11 +592,68 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -267,6 +662,9 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -720,298 +1118,726 @@
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="5">
+      <c r="A10" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="18">
+        <v>145.41</v>
+      </c>
+      <c r="J10" s="18">
+        <v>15.69</v>
+      </c>
+      <c r="K10" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>161.1</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5">
+      <c r="A11" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="18">
+        <v>233.0</v>
+      </c>
+      <c r="J11" s="18">
+        <v>35.0</v>
+      </c>
+      <c r="K11" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5">
+      <c r="A12" s="19">
+        <v>4.0</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="18">
+        <v>8.33</v>
+      </c>
+      <c r="J12" s="18">
+        <v>6.99</v>
+      </c>
+      <c r="K12" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40.31</v>
       </c>
       <c r="L12" s="6"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5">
+      <c r="A13" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="20">
+        <v>1606.0</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="21">
+        <v>1606.0</v>
+      </c>
+      <c r="I13" s="18">
+        <v>5.55</v>
+      </c>
+      <c r="J13" s="18">
+        <v>0.0</v>
+      </c>
+      <c r="K13" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5">
+      <c r="A14" s="19">
+        <v>4.0</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="18">
+        <v>1.95</v>
+      </c>
+      <c r="J14" s="22"/>
+      <c r="K14" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5">
+      <c r="A15" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="18">
+        <v>0.95</v>
+      </c>
+      <c r="J15" s="22"/>
+      <c r="K15" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5">
+      <c r="A16" s="19">
+        <v>3.0</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="J16" s="22"/>
+      <c r="K16" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5">
+      <c r="A17" s="19">
+        <v>3.0</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="J17" s="22"/>
+      <c r="K17" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5">
+      <c r="A18" s="24">
+        <v>2.0</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="26">
+        <v>1729144.0</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="28">
+        <v>1.61</v>
+      </c>
+      <c r="J18" s="29"/>
+      <c r="K18" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5">
+      <c r="A19" s="24">
+        <v>3.0</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="28">
+        <v>0.15</v>
+      </c>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="5">
+      <c r="A20" s="24">
+        <v>10.0</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="J20" s="31"/>
+      <c r="K20" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="5">
+      <c r="A21" s="24">
+        <v>3.0</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="J21" s="31"/>
+      <c r="K21" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="5">
+      <c r="A22" s="24">
+        <v>3.0</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="28">
+        <v>0.11</v>
+      </c>
+      <c r="J22" s="31"/>
+      <c r="K22" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5">
+      <c r="A23" s="24">
+        <v>3.0</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I23" s="28">
+        <v>0.55</v>
+      </c>
+      <c r="J23" s="29"/>
+      <c r="K23" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5">
+      <c r="A24" s="24">
+        <v>3.0</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" s="28">
+        <v>0.53</v>
+      </c>
+      <c r="J24" s="29"/>
+      <c r="K24" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5">
+      <c r="A25" s="24">
+        <v>3.0</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" s="28">
+        <v>0.69</v>
+      </c>
+      <c r="J25" s="29"/>
+      <c r="K25" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.07</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5">
+      <c r="A26" s="24">
+        <v>6.0</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="25">
+        <v>1729128.0</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" s="28">
+        <v>0.79</v>
+      </c>
+      <c r="J26" s="29"/>
+      <c r="K26" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="K27" s="5">
+      <c r="A27" s="32">
+        <v>3.0</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="J27" s="29"/>
+      <c r="K27" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="K28" s="5">
+      <c r="A28" s="32">
+        <v>3.0</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" s="28">
+        <v>0.64</v>
+      </c>
+      <c r="J28" s="29"/>
+      <c r="K28" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="K29" s="5">
+      <c r="A29" s="32">
+        <v>3.0</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="I29" s="28">
+        <v>0.23</v>
+      </c>
+      <c r="J29" s="35"/>
+      <c r="K29" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="K30" s="5">
+      <c r="A30" s="32">
+        <v>3.0</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I30" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="J30" s="35"/>
+      <c r="K30" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
@@ -1057,32 +1883,32 @@
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18">
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37">
         <f>SUM(K7:K26)</f>
-        <v>440.2</v>
+        <v>946.93</v>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="C39" s="4"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>28</v>
+        <v>113</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1101,28 +1927,31 @@
       <c r="K41" s="5"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>31</v>
+      <c r="A42" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" s="40" t="s">
+        <v>117</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="22">
+      <c r="A43" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="42">
         <v>45695.0</v>
       </c>
-      <c r="C43" s="23" t="s">
-        <v>33</v>
+      <c r="C43" s="43" t="s">
+        <v>119</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
@@ -1130,13 +1959,13 @@
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B44" s="22">
+        <v>120</v>
+      </c>
+      <c r="B44" s="42">
         <v>45702.0</v>
       </c>
-      <c r="C44" s="23" t="s">
-        <v>35</v>
+      <c r="C44" s="43" t="s">
+        <v>121</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
@@ -1144,13 +1973,13 @@
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45" s="22">
+        <v>122</v>
+      </c>
+      <c r="B45" s="42">
         <v>45709.0</v>
       </c>
-      <c r="C45" s="23" t="s">
-        <v>37</v>
+      <c r="C45" s="43" t="s">
+        <v>123</v>
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
@@ -1158,13 +1987,13 @@
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" s="22">
+        <v>124</v>
+      </c>
+      <c r="B46" s="42">
         <v>45716.0</v>
       </c>
-      <c r="C46" s="23" t="s">
-        <v>39</v>
+      <c r="C46" s="43" t="s">
+        <v>125</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
@@ -1172,13 +2001,13 @@
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="22">
+        <v>126</v>
+      </c>
+      <c r="B47" s="42">
         <v>45731.0</v>
       </c>
-      <c r="C47" s="23" t="s">
-        <v>41</v>
+      <c r="C47" s="43" t="s">
+        <v>127</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
@@ -1186,19 +2015,28 @@
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="22">
+        <v>128</v>
+      </c>
+      <c r="B48" s="42">
         <v>45732.0</v>
       </c>
-      <c r="C48" s="24" t="s">
-        <v>43</v>
+      <c r="C48" s="44" t="s">
+        <v>129</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
+      <c r="A49" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" s="42">
+        <v>45732.0</v>
+      </c>
+      <c r="C49" s="44" t="s">
+        <v>131</v>
+      </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
@@ -2894,10 +3732,31 @@
     <hyperlink r:id="rId4" ref="H8"/>
     <hyperlink r:id="rId5" ref="E9"/>
     <hyperlink r:id="rId6" ref="H9"/>
+    <hyperlink r:id="rId7" ref="H10"/>
+    <hyperlink r:id="rId8" ref="H11"/>
+    <hyperlink r:id="rId9" ref="H12"/>
+    <hyperlink r:id="rId10" ref="H13"/>
+    <hyperlink r:id="rId11" ref="H14"/>
+    <hyperlink r:id="rId12" ref="H15"/>
+    <hyperlink r:id="rId13" ref="H16"/>
+    <hyperlink r:id="rId14" ref="H17"/>
+    <hyperlink r:id="rId15" ref="H18"/>
+    <hyperlink r:id="rId16" ref="H19"/>
+    <hyperlink r:id="rId17" ref="H20"/>
+    <hyperlink r:id="rId18" ref="H21"/>
+    <hyperlink r:id="rId19" ref="H22"/>
+    <hyperlink r:id="rId20" ref="H23"/>
+    <hyperlink r:id="rId21" ref="H24"/>
+    <hyperlink r:id="rId22" ref="H25"/>
+    <hyperlink r:id="rId23" ref="H26"/>
+    <hyperlink r:id="rId24" ref="H27"/>
+    <hyperlink r:id="rId25" ref="H28"/>
+    <hyperlink r:id="rId26" ref="H29"/>
+    <hyperlink r:id="rId27" ref="H30"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.66666666666667" footer="0.0" header="0.0" left="1.0" right="1.0" top="1.66666666666667"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM to Rev 10
</commit_message>
<xml_diff>
--- a/BOMs/Bill of Materials.xlsx
+++ b/BOMs/Bill of Materials.xlsx
@@ -9,22 +9,38 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="M6GZ3OF3qHAlsWf8pO61Dx1imdDQjCDbbYb+pCm5dgY="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="X6UnsiLNsDpkKMi7G7XgNq64zp/CAMdt6BS4OChi4aE="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="J28">
+      <text>
+        <t xml:space="preserve">
+======</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="222">
   <si>
-    <t>Last modified: 2025-04-02</t>
+    <t>Last modified: 2025-04-11</t>
   </si>
   <si>
-    <t>PCB version: 1</t>
+    <t>Schematic version: 2.0</t>
   </si>
   <si>
-    <t>BOM revision: 8</t>
+    <t>BOM revision: 10</t>
   </si>
   <si>
     <t>P/NP</t>
@@ -354,6 +370,21 @@
     <t>445-8657-1-ND</t>
   </si>
   <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Power Board PCB Cost</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>U8</t>
   </si>
   <si>
@@ -399,9 +430,6 @@
     <t>B0CRVQ4GZ1</t>
   </si>
   <si>
-    <t>ND</t>
-  </si>
-  <si>
     <t>Kxable</t>
   </si>
   <si>
@@ -412,6 +440,183 @@
   </si>
   <si>
     <t>B0BJNZ71K3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	LitStar</t>
+  </si>
+  <si>
+    <t>12V 3A Adapter Power Supply AC to DC Plug 5.5 x 2.1mm &amp; 2.5mm for   3.3ft Cord</t>
+  </si>
+  <si>
+    <t>B08CZ7Z9TB</t>
+  </si>
+  <si>
+    <t>J10, J9</t>
+  </si>
+  <si>
+    <t>Cinch Connectivity Solutions Johnson</t>
+  </si>
+  <si>
+    <t>142-0711-821</t>
+  </si>
+  <si>
+    <t>CONN SMA JACK STR 50OHM EDGE MNT</t>
+  </si>
+  <si>
+    <t>J629-ND</t>
+  </si>
+  <si>
+    <t>Mini-Circuits</t>
+  </si>
+  <si>
+    <t>141-2SM+</t>
+  </si>
+  <si>
+    <t>Cable Assembly Coaxial SMA to SMA Hand Formable .141 2.000" (50.80mm)</t>
+  </si>
+  <si>
+    <t>3157-141-2SM+-ND</t>
+  </si>
+  <si>
+    <t>U15</t>
+  </si>
+  <si>
+    <t>BPF-A1340+</t>
+  </si>
+  <si>
+    <t>RF FILTER BANDPASS 1.34GHZ 18SMD</t>
+  </si>
+  <si>
+    <t>3157-BPF-A1340+CT-ND</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>CL21B104MACNNNC</t>
+  </si>
+  <si>
+    <t>0.1 µF ±20% 25V Ceramic Capacitor X7R 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>1276-2449-1-ND</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>CC0805KRX7R8BB332</t>
+  </si>
+  <si>
+    <t>3300 pF ±10% 25V Ceramic Capacitor X7R 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>311-4318-1-ND</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>CL21A226MQQNNNE</t>
+  </si>
+  <si>
+    <t>22 µF ±20% 6.3V Ceramic Capacitor X5R 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>1276-1100-1-ND</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>Eaton - Electronics Division</t>
+  </si>
+  <si>
+    <t>DRA73-2R2-R</t>
+  </si>
+  <si>
+    <t>FIXED IND 2.2UH 4.18A 16MOHM SMD</t>
+  </si>
+  <si>
+    <t>283-DRA73-2R2-RCT-ND</t>
+  </si>
+  <si>
+    <t>R3,R4</t>
+  </si>
+  <si>
+    <t>RC0805JR-070RL</t>
+  </si>
+  <si>
+    <t>RES 0 OHM JUMPER 1/8W 0805</t>
+  </si>
+  <si>
+    <t>311-0.0ARCT-ND</t>
+  </si>
+  <si>
+    <t>U14</t>
+  </si>
+  <si>
+    <t>TPS62133RGTR</t>
+  </si>
+  <si>
+    <t>Buck Switching Regulator IC Positive Fixed 5V 1 Output 3A 16-VFQFN Exposed Pad</t>
+  </si>
+  <si>
+    <t>296-29937-1-ND</t>
+  </si>
+  <si>
+    <t>SMBJ12A-13-F</t>
+  </si>
+  <si>
+    <t>TVS DIODE 12VWM 19.9VC SMB</t>
+  </si>
+  <si>
+    <t>SMBJ12A-FDICT-ND</t>
+  </si>
+  <si>
+    <t>DMP4047LFDE-7</t>
+  </si>
+  <si>
+    <t>MOSFET P-CH 40V 3.3A 6UDFN</t>
+  </si>
+  <si>
+    <t>DMP4047LFDE-7DITR-ND</t>
+  </si>
+  <si>
+    <t>MAX8510EXK30+T</t>
+  </si>
+  <si>
+    <t>Analog Devices Inc./Maxim Integrated</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3V 120MA SC-70-5</t>
+  </si>
+  <si>
+    <t>MAX8510EXK30+TCT-ND</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C5, C7</t>
+  </si>
+  <si>
+    <t>CC0805JKX7R8BB105</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 25V X7R 0805</t>
+  </si>
+  <si>
+    <t>13-CC0805JKX7R8BB105CT-ND</t>
+  </si>
+  <si>
+    <t>GRM2195C1H103JA01D</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 50V C0G/NP0 0805</t>
+  </si>
+  <si>
+    <t>490-1642-1-ND</t>
   </si>
   <si>
     <t>TOTAL:</t>
@@ -438,10 +643,16 @@
     <t>First Draft of Inclusive BOM, Added LNA.</t>
   </si>
   <si>
+    <t>PoE</t>
+  </si>
+  <si>
     <t>v2.0</t>
   </si>
   <si>
     <t>Added SDR (MISSING SHIPPING COST)</t>
+  </si>
+  <si>
+    <t>RF Board</t>
   </si>
   <si>
     <t>v3.0</t>
@@ -474,10 +685,19 @@
     <t>Ordered Power Management Board, N Connectors, and Filter Board IC's</t>
   </si>
   <si>
-    <t>v8.0</t>
+    <t>V8.0</t>
   </si>
   <si>
     <t>Ordered PoE Parts through Amazon</t>
+  </si>
+  <si>
+    <t>V9.0</t>
+  </si>
+  <si>
+    <t>V10.0</t>
+  </si>
+  <si>
+    <t>Updated Components Bought in 2nd DigiKey Order</t>
   </si>
 </sst>
 </file>
@@ -488,7 +708,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -502,10 +722,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Serif"/>
     </font>
     <font>
       <b/>
@@ -538,17 +754,16 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <sz val="9.0"/>
+      <color rgb="FF222222"/>
+      <name val="Roboto"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,14 +778,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
+        <fgColor rgb="FF1155CC"/>
+        <bgColor rgb="FF1155CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -583,103 +810,103 @@
       <bottom/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF0000FF"/>
+        <color rgb="FF000000"/>
       </left>
       <top style="thin">
-        <color rgb="FF0000FF"/>
+        <color rgb="FF000000"/>
       </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <bottom style="thin">
-        <color rgb="FF0000FF"/>
+        <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF1155CC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF1155CC"/>
+      </right>
       <top style="thin">
-        <color rgb="FF0000FF"/>
+        <color rgb="FF1155CC"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF0000FF"/>
+        <color rgb="FF1155CC"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="FFFFFF00"/>
       </left>
-      <top style="thin">
-        <color rgb="FFFFFF00"/>
-      </top>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FFFFFF00"/>
-      </top>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FFFFFF00"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD5D9D9"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FFFFFF00"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFF00"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFF00"/>
-      </left>
-    </border>
-    <border>
       <right style="thin">
         <color rgb="FFFFFF00"/>
       </right>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFF00"/>
-      </left>
-      <bottom style="thin">
-        <color rgb="FFFFFF00"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color rgb="FFFFFF00"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FFFFFF00"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FFFFFF00"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF0000FF"/>
+        <color rgb="FFFF0000"/>
       </left>
       <right style="thin">
-        <color rgb="FF0000FF"/>
+        <color rgb="FFFF0000"/>
       </right>
       <top style="thin">
-        <color rgb="FF0000FF"/>
+        <color rgb="FFFF0000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF0000FF"/>
+        <color rgb="FFFF0000"/>
       </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -701,17 +928,32 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -722,10 +964,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -734,82 +976,85 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -821,7 +1066,19 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1055,9 +1312,9 @@
     <col customWidth="1" min="1" max="1" width="5.14"/>
     <col customWidth="1" min="2" max="2" width="30.71"/>
     <col customWidth="1" min="3" max="3" width="5.71"/>
-    <col customWidth="1" min="4" max="4" width="23.71"/>
-    <col customWidth="1" min="5" max="5" width="26.43"/>
-    <col customWidth="1" min="6" max="6" width="75.0"/>
+    <col customWidth="1" min="4" max="4" width="38.0"/>
+    <col customWidth="1" min="5" max="5" width="30.57"/>
+    <col customWidth="1" min="6" max="6" width="75.57"/>
     <col customWidth="1" min="7" max="7" width="19.43"/>
     <col customWidth="1" min="8" max="8" width="24.29"/>
     <col customWidth="1" min="9" max="11" width="8.71"/>
@@ -1124,7 +1381,7 @@
       <c r="AA2" s="3"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
@@ -1162,7 +1419,7 @@
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="3"/>
@@ -1219,37 +1476,37 @@
       <c r="AA5" s="3"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="3"/>
@@ -1270,7 +1527,7 @@
       <c r="AA6" s="3"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>1.0</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -1300,8 +1557,8 @@
       <c r="J7" s="13">
         <v>15.69</v>
       </c>
-      <c r="K7" s="13">
-        <f t="shared" ref="K7:K37" si="1">(A7*I7)+J7</f>
+      <c r="K7" s="14">
+        <f t="shared" ref="K7:K47" si="1">(A7*I7)+J7</f>
         <v>161.1</v>
       </c>
       <c r="L7" s="3"/>
@@ -1322,37 +1579,37 @@
       <c r="AA7" s="3"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="11">
+      <c r="A8" s="15">
         <v>1.0</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="18">
         <v>233.0</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="18">
         <v>35.0</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="19">
         <f t="shared" si="1"/>
         <v>268</v>
       </c>
@@ -1374,37 +1631,37 @@
       <c r="AA8" s="3"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="11">
+      <c r="A9" s="15">
         <v>3.0</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="17">
         <v>1606.0</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="17">
         <v>1606.0</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="18">
         <v>5.55</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="18">
         <v>0.0</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="19">
         <f t="shared" si="1"/>
         <v>16.65</v>
       </c>
@@ -1426,37 +1683,37 @@
       <c r="AA9" s="3"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="14">
+      <c r="A10" s="15">
         <v>4.0</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="18">
         <v>8.33</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="18">
         <v>6.99</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="19">
         <f t="shared" si="1"/>
         <v>40.31</v>
       </c>
@@ -1478,35 +1735,35 @@
       <c r="AA10" s="3"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="15">
+      <c r="A11" s="20">
         <v>4.0</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="18">
         <v>1.95</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13">
+      <c r="J11" s="18"/>
+      <c r="K11" s="19">
         <f t="shared" si="1"/>
         <v>7.8</v>
       </c>
@@ -1528,35 +1785,35 @@
       <c r="AA11" s="3"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="15">
+      <c r="A12" s="20">
         <v>2.0</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="18">
         <v>0.95</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13">
+      <c r="J12" s="18"/>
+      <c r="K12" s="19">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
@@ -1578,35 +1835,35 @@
       <c r="AA12" s="3"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="15">
+      <c r="A13" s="20">
         <v>3.0</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="18">
         <v>0.12</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13">
+      <c r="J13" s="18"/>
+      <c r="K13" s="19">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
@@ -1628,35 +1885,35 @@
       <c r="AA13" s="3"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="15">
+      <c r="A14" s="20">
         <v>3.0</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="18">
         <v>0.12</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13">
+      <c r="J14" s="18"/>
+      <c r="K14" s="19">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
@@ -1678,35 +1935,35 @@
       <c r="AA14" s="3"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="18">
+      <c r="A15" s="23">
         <v>2.0</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="21">
         <v>1729144.0</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="18">
         <v>1.61</v>
       </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="13">
+      <c r="J15" s="18"/>
+      <c r="K15" s="19">
         <f t="shared" si="1"/>
         <v>3.22</v>
       </c>
@@ -1728,35 +1985,35 @@
       <c r="AA15" s="3"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="18">
+      <c r="A16" s="23">
         <v>3.0</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="18">
         <v>0.15</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="13">
+      <c r="J16" s="18"/>
+      <c r="K16" s="19">
         <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
@@ -1778,35 +2035,35 @@
       <c r="AA16" s="3"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="18">
+      <c r="A17" s="23">
         <v>10.0</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="18">
         <v>0.1</v>
       </c>
-      <c r="J17" s="21"/>
-      <c r="K17" s="13">
+      <c r="J17" s="18"/>
+      <c r="K17" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1828,35 +2085,35 @@
       <c r="AA17" s="3"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="18">
+      <c r="A18" s="23">
         <v>3.0</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="18">
         <v>0.25</v>
       </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="13">
+      <c r="J18" s="18"/>
+      <c r="K18" s="19">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
@@ -1878,35 +2135,35 @@
       <c r="AA18" s="3"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="18">
+      <c r="A19" s="23">
         <v>3.0</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="18">
         <v>0.11</v>
       </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="13">
+      <c r="J19" s="18"/>
+      <c r="K19" s="19">
         <f t="shared" si="1"/>
         <v>0.33</v>
       </c>
@@ -1928,35 +2185,35 @@
       <c r="AA19" s="3"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="18">
+      <c r="A20" s="23">
         <v>3.0</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="I20" s="21">
+      <c r="I20" s="18">
         <v>0.55</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="13">
+      <c r="J20" s="18"/>
+      <c r="K20" s="19">
         <f t="shared" si="1"/>
         <v>1.65</v>
       </c>
@@ -1978,35 +2235,35 @@
       <c r="AA20" s="3"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="18">
+      <c r="A21" s="23">
         <v>3.0</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="18">
         <v>0.53</v>
       </c>
-      <c r="J21" s="21"/>
-      <c r="K21" s="13">
+      <c r="J21" s="18"/>
+      <c r="K21" s="19">
         <f t="shared" si="1"/>
         <v>1.59</v>
       </c>
@@ -2028,35 +2285,35 @@
       <c r="AA21" s="3"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="18">
+      <c r="A22" s="23">
         <v>3.0</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="I22" s="21">
+      <c r="I22" s="18">
         <v>0.69</v>
       </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="13">
+      <c r="J22" s="18"/>
+      <c r="K22" s="19">
         <f t="shared" si="1"/>
         <v>2.07</v>
       </c>
@@ -2078,35 +2335,35 @@
       <c r="AA22" s="3"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="18">
+      <c r="A23" s="23">
         <v>6.0</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="21">
         <v>1729128.0</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="I23" s="21">
+      <c r="I23" s="18">
         <v>0.79</v>
       </c>
-      <c r="J23" s="21"/>
-      <c r="K23" s="13">
+      <c r="J23" s="18"/>
+      <c r="K23" s="19">
         <f t="shared" si="1"/>
         <v>4.74</v>
       </c>
@@ -2128,35 +2385,35 @@
       <c r="AA23" s="3"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="18">
+      <c r="A24" s="23">
         <v>3.0</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="I24" s="21">
+      <c r="I24" s="18">
         <v>0.1</v>
       </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="13">
+      <c r="J24" s="18"/>
+      <c r="K24" s="19">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
@@ -2178,35 +2435,35 @@
       <c r="AA24" s="3"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="18">
+      <c r="A25" s="23">
         <v>3.0</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="H25" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="I25" s="21">
+      <c r="I25" s="18">
         <v>0.64</v>
       </c>
-      <c r="J25" s="21"/>
-      <c r="K25" s="13">
+      <c r="J25" s="18"/>
+      <c r="K25" s="19">
         <f t="shared" si="1"/>
         <v>1.92</v>
       </c>
@@ -2228,35 +2485,35 @@
       <c r="AA25" s="3"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="18">
+      <c r="A26" s="23">
         <v>3.0</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="F26" s="19" t="s">
+      <c r="F26" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I26" s="21">
+      <c r="I26" s="18">
         <v>0.23</v>
       </c>
-      <c r="J26" s="21"/>
-      <c r="K26" s="13">
+      <c r="J26" s="18"/>
+      <c r="K26" s="19">
         <f t="shared" si="1"/>
         <v>0.69</v>
       </c>
@@ -2278,35 +2535,35 @@
       <c r="AA26" s="3"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="24">
+      <c r="A27" s="25">
         <v>3.0</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="25" t="s">
+      <c r="H27" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="I27" s="21">
+      <c r="I27" s="18">
         <v>0.1</v>
       </c>
-      <c r="J27" s="21"/>
-      <c r="K27" s="13">
+      <c r="J27" s="18"/>
+      <c r="K27" s="19">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
@@ -2328,37 +2585,39 @@
       <c r="AA27" s="3"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="26">
+      <c r="A28" s="27">
         <v>1.0</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="E28" s="27">
-        <v>6.34475546338E11</v>
-      </c>
-      <c r="F28" s="27" t="s">
+      <c r="E28" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="27" t="s">
+      <c r="F28" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="H28" s="28" t="s">
+      <c r="G28" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H28" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="I28" s="29">
-        <v>9.99</v>
-      </c>
-      <c r="J28" s="30"/>
-      <c r="K28" s="13">
+      <c r="I28" s="28">
+        <v>3.2</v>
+      </c>
+      <c r="J28" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="K28" s="19">
         <f t="shared" si="1"/>
-        <v>9.99</v>
+        <v>4.7</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -2378,37 +2637,37 @@
       <c r="AA28" s="3"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="31">
+      <c r="A29" s="29">
         <v>1.0</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="D29" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="24">
+        <v>6.34475546338E11</v>
+      </c>
+      <c r="F29" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="F29" s="32" t="s">
+      <c r="G29" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="H29" s="33" t="s">
+      <c r="H29" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="I29" s="13">
-        <v>16.99</v>
-      </c>
-      <c r="J29" s="34"/>
-      <c r="K29" s="13">
+      <c r="I29" s="18">
+        <v>9.99</v>
+      </c>
+      <c r="J29" s="18"/>
+      <c r="K29" s="19">
         <f t="shared" si="1"/>
-        <v>16.99</v>
+        <v>9.99</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -2428,37 +2687,37 @@
       <c r="AA29" s="3"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="31">
+      <c r="A30" s="29">
         <v>1.0</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="G30" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="H30" s="33" t="s">
+      <c r="G30" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H30" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="I30" s="13">
-        <v>21.99</v>
-      </c>
-      <c r="J30" s="34"/>
-      <c r="K30" s="13">
+      <c r="I30" s="18">
+        <v>16.99</v>
+      </c>
+      <c r="J30" s="18"/>
+      <c r="K30" s="19">
         <f t="shared" si="1"/>
-        <v>21.99</v>
+        <v>16.99</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -2478,37 +2737,37 @@
       <c r="AA30" s="3"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="35">
+      <c r="A31" s="29">
         <v>1.0</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="E31" s="36" t="s">
+      <c r="E31" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="F31" s="36" t="s">
+      <c r="F31" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="G31" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="H31" s="37" t="s">
+      <c r="G31" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H31" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="I31" s="38">
-        <v>8.49</v>
-      </c>
-      <c r="J31" s="39"/>
-      <c r="K31" s="13">
+      <c r="I31" s="18">
+        <v>21.99</v>
+      </c>
+      <c r="J31" s="18"/>
+      <c r="K31" s="19">
         <f t="shared" si="1"/>
-        <v>8.49</v>
+        <v>21.99</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -2528,19 +2787,37 @@
       <c r="AA31" s="3"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="32"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="13">
+      <c r="A32" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H32" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="I32" s="18">
+        <v>8.49</v>
+      </c>
+      <c r="J32" s="18"/>
+      <c r="K32" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.49</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -2560,19 +2837,37 @@
       <c r="AA32" s="3"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="32"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="13">
+      <c r="A33" s="31">
+        <v>1.0</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="I33" s="18">
+        <v>9.99</v>
+      </c>
+      <c r="J33" s="24"/>
+      <c r="K33" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.99</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2592,19 +2887,39 @@
       <c r="AA33" s="3"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="13">
+      <c r="A34" s="32">
+        <v>3.0</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="I34" s="33">
+        <v>6.64</v>
+      </c>
+      <c r="J34" s="34">
+        <v>12.99</v>
+      </c>
+      <c r="K34" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>32.91</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -2624,19 +2939,37 @@
       <c r="AA34" s="3"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="13">
+      <c r="A35" s="32">
+        <v>3.0</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="I35" s="18">
+        <v>16.26</v>
+      </c>
+      <c r="J35" s="24"/>
+      <c r="K35" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>48.78</v>
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -2656,19 +2989,37 @@
       <c r="AA35" s="3"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="13">
+      <c r="A36" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="I36" s="36">
+        <v>71.27</v>
+      </c>
+      <c r="J36" s="24"/>
+      <c r="K36" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>71.27</v>
       </c>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -2688,19 +3039,37 @@
       <c r="AA36" s="3"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="13">
+      <c r="A37" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="G37" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="I37" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="J37" s="18"/>
+      <c r="K37" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -2720,21 +3089,37 @@
       <c r="AA37" s="3"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="J38" s="6"/>
-      <c r="K38" s="41">
-        <f>SUM(K7:K37)</f>
-        <v>572.95</v>
+      <c r="A38" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="G38" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="I38" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="J38" s="24"/>
+      <c r="K38" s="19">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -2754,17 +3139,38 @@
       <c r="AA38" s="3"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
+      <c r="A39" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="G39" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="I39" s="38">
+        <v>0.12</v>
+      </c>
+      <c r="J39" s="24"/>
+      <c r="K39" s="19">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -2783,19 +3189,38 @@
       <c r="AA39" s="3"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+      <c r="A40" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="E40" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="F40" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G40" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="I40" s="38">
+        <v>1.75</v>
+      </c>
+      <c r="J40" s="24"/>
+      <c r="K40" s="19">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -2814,17 +3239,38 @@
       <c r="AA40" s="3"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
+      <c r="A41" s="25">
+        <v>10.0</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="J41" s="24"/>
+      <c r="K41" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -2843,25 +3289,38 @@
       <c r="AA41" s="3"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B42" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C42" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
+      <c r="A42" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="G42" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="I42" s="38">
+        <v>1.71</v>
+      </c>
+      <c r="J42" s="24"/>
+      <c r="K42" s="19">
+        <f t="shared" si="1"/>
+        <v>3.42</v>
+      </c>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -2880,23 +3339,38 @@
       <c r="AA42" s="3"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="B43" s="45">
-        <v>45695.0</v>
-      </c>
-      <c r="C43" s="46" t="s">
-        <v>139</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
+      <c r="A43" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="G43" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H43" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="I43" s="38">
+        <v>0.26</v>
+      </c>
+      <c r="J43" s="24"/>
+      <c r="K43" s="19">
+        <f t="shared" si="1"/>
+        <v>0.78</v>
+      </c>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -2915,23 +3389,38 @@
       <c r="AA43" s="3"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="B44" s="45">
-        <v>45702.0</v>
-      </c>
-      <c r="C44" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
+      <c r="A44" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="G44" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H44" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="I44" s="38">
+        <v>0.74</v>
+      </c>
+      <c r="J44" s="24"/>
+      <c r="K44" s="19">
+        <f t="shared" si="1"/>
+        <v>2.22</v>
+      </c>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
@@ -2950,23 +3439,38 @@
       <c r="AA44" s="3"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="B45" s="45">
-        <v>45709.0</v>
-      </c>
-      <c r="C45" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
+      <c r="A45" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="G45" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H45" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="I45" s="38">
+        <v>1.84</v>
+      </c>
+      <c r="J45" s="24"/>
+      <c r="K45" s="19">
+        <f t="shared" si="1"/>
+        <v>3.68</v>
+      </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -2985,23 +3489,38 @@
       <c r="AA45" s="3"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="B46" s="45">
-        <v>45716.0</v>
-      </c>
-      <c r="C46" s="46" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
+      <c r="A46" s="25">
+        <v>12.0</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H46" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="I46" s="39">
+        <v>0.07</v>
+      </c>
+      <c r="J46" s="24"/>
+      <c r="K46" s="19">
+        <f t="shared" si="1"/>
+        <v>0.84</v>
+      </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -3020,23 +3539,38 @@
       <c r="AA46" s="3"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="B47" s="45">
-        <v>45731.0</v>
-      </c>
-      <c r="C47" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
+      <c r="A47" s="25">
+        <v>5.0</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="G47" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H47" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="I47" s="39">
+        <v>0.18</v>
+      </c>
+      <c r="J47" s="24"/>
+      <c r="K47" s="19">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -3055,23 +3589,17 @@
       <c r="AA47" s="3"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="A48" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="B48" s="45">
-        <v>45732.0</v>
-      </c>
-      <c r="C48" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
+      <c r="A48" s="40"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="19"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -3090,23 +3618,22 @@
       <c r="AA48" s="3"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="46" t="s">
-        <v>150</v>
-      </c>
-      <c r="B49" s="45">
-        <v>45732.0</v>
-      </c>
-      <c r="C49" s="46" t="s">
-        <v>151</v>
-      </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="J49" s="44"/>
+      <c r="K49" s="45">
+        <f>SUM(K7:K47)</f>
+        <v>757.9</v>
+      </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -3125,15 +3652,9 @@
       <c r="AA49" s="3"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="B50" s="49">
-        <v>45749.0</v>
-      </c>
-      <c r="C50" s="48" t="s">
-        <v>153</v>
-      </c>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="5"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -3160,17 +3681,19 @@
       <c r="AA50" s="3"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="3"/>
-      <c r="B51" s="50"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
+      <c r="A51" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -3190,7 +3713,7 @@
     </row>
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" s="3"/>
-      <c r="B52" s="50"/>
+      <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -3218,13 +3741,21 @@
       <c r="AA52" s="3"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="3"/>
-      <c r="B53" s="50"/>
-      <c r="C53" s="3"/>
+      <c r="A53" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="B53" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="C53" s="47" t="s">
+        <v>199</v>
+      </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="48" t="s">
+        <v>200</v>
+      </c>
+      <c r="G53" s="49"/>
       <c r="H53" s="3"/>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
@@ -3247,13 +3778,21 @@
       <c r="AA53" s="3"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="3"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="3"/>
+      <c r="A54" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="B54" s="51">
+        <v>45695.0</v>
+      </c>
+      <c r="C54" s="52" t="s">
+        <v>202</v>
+      </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
+      <c r="F54" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="G54" s="54"/>
       <c r="H54" s="3"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
@@ -3276,13 +3815,21 @@
       <c r="AA54" s="3"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
+      <c r="A55" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="B55" s="51">
+        <v>45702.0</v>
+      </c>
+      <c r="C55" s="52" t="s">
+        <v>205</v>
+      </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
+      <c r="F55" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="G55" s="57"/>
       <c r="H55" s="3"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
@@ -3305,9 +3852,15 @@
       <c r="AA55" s="3"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
+      <c r="A56" s="55" t="s">
+        <v>207</v>
+      </c>
+      <c r="B56" s="51">
+        <v>45709.0</v>
+      </c>
+      <c r="C56" s="52" t="s">
+        <v>208</v>
+      </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -3334,9 +3887,15 @@
       <c r="AA56" s="3"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
+      <c r="A57" s="55" t="s">
+        <v>209</v>
+      </c>
+      <c r="B57" s="51">
+        <v>45716.0</v>
+      </c>
+      <c r="C57" s="52" t="s">
+        <v>210</v>
+      </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -3363,9 +3922,15 @@
       <c r="AA57" s="3"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
+      <c r="A58" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="B58" s="51">
+        <v>45731.0</v>
+      </c>
+      <c r="C58" s="52" t="s">
+        <v>212</v>
+      </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -3392,9 +3957,15 @@
       <c r="AA58" s="3"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
+      <c r="A59" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="B59" s="51">
+        <v>45732.0</v>
+      </c>
+      <c r="C59" s="52" t="s">
+        <v>214</v>
+      </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -3421,9 +3992,15 @@
       <c r="AA59" s="3"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
+      <c r="A60" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="B60" s="51">
+        <v>45732.0</v>
+      </c>
+      <c r="C60" s="52" t="s">
+        <v>216</v>
+      </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -3450,9 +4027,15 @@
       <c r="AA60" s="3"/>
     </row>
     <row r="61" ht="12.75" customHeight="1">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
+      <c r="A61" s="58" t="s">
+        <v>217</v>
+      </c>
+      <c r="B61" s="59">
+        <v>45749.0</v>
+      </c>
+      <c r="C61" s="58" t="s">
+        <v>218</v>
+      </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -3479,9 +4062,15 @@
       <c r="AA61" s="3"/>
     </row>
     <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
+      <c r="A62" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="B62" s="59">
+        <v>45751.0</v>
+      </c>
+      <c r="C62" s="58" t="s">
+        <v>218</v>
+      </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -3508,9 +4097,15 @@
       <c r="AA62" s="3"/>
     </row>
     <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
+      <c r="A63" s="58" t="s">
+        <v>220</v>
+      </c>
+      <c r="B63" s="59">
+        <v>45758.0</v>
+      </c>
+      <c r="C63" s="58" t="s">
+        <v>221</v>
+      </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -3538,7 +4133,7 @@
     </row>
     <row r="64" ht="12.75" customHeight="1">
       <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
+      <c r="B64" s="60"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -3567,7 +4162,7 @@
     </row>
     <row r="65" ht="12.75" customHeight="1">
       <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
+      <c r="B65" s="60"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -8437,7 +9032,7 @@
       <c r="Z232" s="3"/>
       <c r="AA232" s="3"/>
     </row>
-    <row r="233" ht="15.75" customHeight="1">
+    <row r="233" ht="12.75" customHeight="1">
       <c r="A233" s="3"/>
       <c r="B233" s="3"/>
       <c r="C233" s="3"/>
@@ -8466,7 +9061,7 @@
       <c r="Z233" s="3"/>
       <c r="AA233" s="3"/>
     </row>
-    <row r="234" ht="15.75" customHeight="1">
+    <row r="234" ht="12.75" customHeight="1">
       <c r="A234" s="3"/>
       <c r="B234" s="3"/>
       <c r="C234" s="3"/>
@@ -8495,7 +9090,7 @@
       <c r="Z234" s="3"/>
       <c r="AA234" s="3"/>
     </row>
-    <row r="235" ht="15.75" customHeight="1">
+    <row r="235" ht="12.75" customHeight="1">
       <c r="A235" s="3"/>
       <c r="B235" s="3"/>
       <c r="C235" s="3"/>
@@ -8524,7 +9119,7 @@
       <c r="Z235" s="3"/>
       <c r="AA235" s="3"/>
     </row>
-    <row r="236" ht="15.75" customHeight="1">
+    <row r="236" ht="12.75" customHeight="1">
       <c r="A236" s="3"/>
       <c r="B236" s="3"/>
       <c r="C236" s="3"/>
@@ -8553,7 +9148,7 @@
       <c r="Z236" s="3"/>
       <c r="AA236" s="3"/>
     </row>
-    <row r="237" ht="15.75" customHeight="1">
+    <row r="237" ht="12.75" customHeight="1">
       <c r="A237" s="3"/>
       <c r="B237" s="3"/>
       <c r="C237" s="3"/>
@@ -8582,7 +9177,7 @@
       <c r="Z237" s="3"/>
       <c r="AA237" s="3"/>
     </row>
-    <row r="238" ht="15.75" customHeight="1">
+    <row r="238" ht="12.75" customHeight="1">
       <c r="A238" s="3"/>
       <c r="B238" s="3"/>
       <c r="C238" s="3"/>
@@ -8591,9 +9186,9 @@
       <c r="F238" s="3"/>
       <c r="G238" s="3"/>
       <c r="H238" s="3"/>
-      <c r="I238" s="3"/>
-      <c r="J238" s="3"/>
-      <c r="K238" s="3"/>
+      <c r="I238" s="6"/>
+      <c r="J238" s="6"/>
+      <c r="K238" s="6"/>
       <c r="L238" s="3"/>
       <c r="M238" s="3"/>
       <c r="N238" s="3"/>
@@ -8611,7 +9206,7 @@
       <c r="Z238" s="3"/>
       <c r="AA238" s="3"/>
     </row>
-    <row r="239" ht="15.75" customHeight="1">
+    <row r="239" ht="12.75" customHeight="1">
       <c r="A239" s="3"/>
       <c r="B239" s="3"/>
       <c r="C239" s="3"/>
@@ -8620,9 +9215,9 @@
       <c r="F239" s="3"/>
       <c r="G239" s="3"/>
       <c r="H239" s="3"/>
-      <c r="I239" s="3"/>
-      <c r="J239" s="3"/>
-      <c r="K239" s="3"/>
+      <c r="I239" s="6"/>
+      <c r="J239" s="6"/>
+      <c r="K239" s="6"/>
       <c r="L239" s="3"/>
       <c r="M239" s="3"/>
       <c r="N239" s="3"/>
@@ -8640,7 +9235,7 @@
       <c r="Z239" s="3"/>
       <c r="AA239" s="3"/>
     </row>
-    <row r="240" ht="15.75" customHeight="1">
+    <row r="240" ht="12.75" customHeight="1">
       <c r="A240" s="3"/>
       <c r="B240" s="3"/>
       <c r="C240" s="3"/>
@@ -8649,9 +9244,9 @@
       <c r="F240" s="3"/>
       <c r="G240" s="3"/>
       <c r="H240" s="3"/>
-      <c r="I240" s="3"/>
-      <c r="J240" s="3"/>
-      <c r="K240" s="3"/>
+      <c r="I240" s="6"/>
+      <c r="J240" s="6"/>
+      <c r="K240" s="6"/>
       <c r="L240" s="3"/>
       <c r="M240" s="3"/>
       <c r="N240" s="3"/>
@@ -8669,7 +9264,7 @@
       <c r="Z240" s="3"/>
       <c r="AA240" s="3"/>
     </row>
-    <row r="241" ht="15.75" customHeight="1">
+    <row r="241" ht="12.75" customHeight="1">
       <c r="A241" s="3"/>
       <c r="B241" s="3"/>
       <c r="C241" s="3"/>
@@ -8678,9 +9273,9 @@
       <c r="F241" s="3"/>
       <c r="G241" s="3"/>
       <c r="H241" s="3"/>
-      <c r="I241" s="3"/>
-      <c r="J241" s="3"/>
-      <c r="K241" s="3"/>
+      <c r="I241" s="6"/>
+      <c r="J241" s="6"/>
+      <c r="K241" s="6"/>
       <c r="L241" s="3"/>
       <c r="M241" s="3"/>
       <c r="N241" s="3"/>
@@ -8698,7 +9293,7 @@
       <c r="Z241" s="3"/>
       <c r="AA241" s="3"/>
     </row>
-    <row r="242" ht="15.75" customHeight="1">
+    <row r="242" ht="12.75" customHeight="1">
       <c r="A242" s="3"/>
       <c r="B242" s="3"/>
       <c r="C242" s="3"/>
@@ -8707,9 +9302,9 @@
       <c r="F242" s="3"/>
       <c r="G242" s="3"/>
       <c r="H242" s="3"/>
-      <c r="I242" s="3"/>
-      <c r="J242" s="3"/>
-      <c r="K242" s="3"/>
+      <c r="I242" s="6"/>
+      <c r="J242" s="6"/>
+      <c r="K242" s="6"/>
       <c r="L242" s="3"/>
       <c r="M242" s="3"/>
       <c r="N242" s="3"/>
@@ -8727,7 +9322,7 @@
       <c r="Z242" s="3"/>
       <c r="AA242" s="3"/>
     </row>
-    <row r="243" ht="15.75" customHeight="1">
+    <row r="243" ht="12.75" customHeight="1">
       <c r="A243" s="3"/>
       <c r="B243" s="3"/>
       <c r="C243" s="3"/>
@@ -8736,9 +9331,9 @@
       <c r="F243" s="3"/>
       <c r="G243" s="3"/>
       <c r="H243" s="3"/>
-      <c r="I243" s="3"/>
-      <c r="J243" s="3"/>
-      <c r="K243" s="3"/>
+      <c r="I243" s="6"/>
+      <c r="J243" s="6"/>
+      <c r="K243" s="6"/>
       <c r="L243" s="3"/>
       <c r="M243" s="3"/>
       <c r="N243" s="3"/>
@@ -8765,9 +9360,9 @@
       <c r="F244" s="3"/>
       <c r="G244" s="3"/>
       <c r="H244" s="3"/>
-      <c r="I244" s="3"/>
-      <c r="J244" s="3"/>
-      <c r="K244" s="3"/>
+      <c r="I244" s="6"/>
+      <c r="J244" s="6"/>
+      <c r="K244" s="6"/>
       <c r="L244" s="3"/>
       <c r="M244" s="3"/>
       <c r="N244" s="3"/>
@@ -8794,9 +9389,9 @@
       <c r="F245" s="3"/>
       <c r="G245" s="3"/>
       <c r="H245" s="3"/>
-      <c r="I245" s="3"/>
-      <c r="J245" s="3"/>
-      <c r="K245" s="3"/>
+      <c r="I245" s="6"/>
+      <c r="J245" s="6"/>
+      <c r="K245" s="6"/>
       <c r="L245" s="3"/>
       <c r="M245" s="3"/>
       <c r="N245" s="3"/>
@@ -8823,9 +9418,9 @@
       <c r="F246" s="3"/>
       <c r="G246" s="3"/>
       <c r="H246" s="3"/>
-      <c r="I246" s="3"/>
-      <c r="J246" s="3"/>
-      <c r="K246" s="3"/>
+      <c r="I246" s="6"/>
+      <c r="J246" s="6"/>
+      <c r="K246" s="6"/>
       <c r="L246" s="3"/>
       <c r="M246" s="3"/>
       <c r="N246" s="3"/>
@@ -8852,9 +9447,9 @@
       <c r="F247" s="3"/>
       <c r="G247" s="3"/>
       <c r="H247" s="3"/>
-      <c r="I247" s="3"/>
-      <c r="J247" s="3"/>
-      <c r="K247" s="3"/>
+      <c r="I247" s="6"/>
+      <c r="J247" s="6"/>
+      <c r="K247" s="6"/>
       <c r="L247" s="3"/>
       <c r="M247" s="3"/>
       <c r="N247" s="3"/>
@@ -8881,9 +9476,9 @@
       <c r="F248" s="3"/>
       <c r="G248" s="3"/>
       <c r="H248" s="3"/>
-      <c r="I248" s="3"/>
-      <c r="J248" s="3"/>
-      <c r="K248" s="3"/>
+      <c r="I248" s="6"/>
+      <c r="J248" s="6"/>
+      <c r="K248" s="6"/>
       <c r="L248" s="3"/>
       <c r="M248" s="3"/>
       <c r="N248" s="3"/>
@@ -30854,43 +31449,378 @@
       <c r="Z1005" s="3"/>
       <c r="AA1005" s="3"/>
     </row>
+    <row r="1006" ht="15.75" customHeight="1">
+      <c r="A1006" s="3"/>
+      <c r="B1006" s="3"/>
+      <c r="C1006" s="3"/>
+      <c r="D1006" s="3"/>
+      <c r="E1006" s="3"/>
+      <c r="F1006" s="3"/>
+      <c r="G1006" s="3"/>
+      <c r="H1006" s="3"/>
+      <c r="I1006" s="3"/>
+      <c r="J1006" s="3"/>
+      <c r="K1006" s="3"/>
+      <c r="L1006" s="3"/>
+      <c r="M1006" s="3"/>
+      <c r="N1006" s="3"/>
+      <c r="O1006" s="3"/>
+      <c r="P1006" s="3"/>
+      <c r="Q1006" s="3"/>
+      <c r="R1006" s="3"/>
+      <c r="S1006" s="3"/>
+      <c r="T1006" s="3"/>
+      <c r="U1006" s="3"/>
+      <c r="V1006" s="3"/>
+      <c r="W1006" s="3"/>
+      <c r="X1006" s="3"/>
+      <c r="Y1006" s="3"/>
+      <c r="Z1006" s="3"/>
+      <c r="AA1006" s="3"/>
+    </row>
+    <row r="1007" ht="15.75" customHeight="1">
+      <c r="A1007" s="3"/>
+      <c r="B1007" s="3"/>
+      <c r="C1007" s="3"/>
+      <c r="D1007" s="3"/>
+      <c r="E1007" s="3"/>
+      <c r="F1007" s="3"/>
+      <c r="G1007" s="3"/>
+      <c r="H1007" s="3"/>
+      <c r="I1007" s="3"/>
+      <c r="J1007" s="3"/>
+      <c r="K1007" s="3"/>
+      <c r="L1007" s="3"/>
+      <c r="M1007" s="3"/>
+      <c r="N1007" s="3"/>
+      <c r="O1007" s="3"/>
+      <c r="P1007" s="3"/>
+      <c r="Q1007" s="3"/>
+      <c r="R1007" s="3"/>
+      <c r="S1007" s="3"/>
+      <c r="T1007" s="3"/>
+      <c r="U1007" s="3"/>
+      <c r="V1007" s="3"/>
+      <c r="W1007" s="3"/>
+      <c r="X1007" s="3"/>
+      <c r="Y1007" s="3"/>
+      <c r="Z1007" s="3"/>
+      <c r="AA1007" s="3"/>
+    </row>
+    <row r="1008" ht="15.75" customHeight="1">
+      <c r="A1008" s="3"/>
+      <c r="B1008" s="3"/>
+      <c r="C1008" s="3"/>
+      <c r="D1008" s="3"/>
+      <c r="E1008" s="3"/>
+      <c r="F1008" s="3"/>
+      <c r="G1008" s="3"/>
+      <c r="H1008" s="3"/>
+      <c r="I1008" s="3"/>
+      <c r="J1008" s="3"/>
+      <c r="K1008" s="3"/>
+      <c r="L1008" s="3"/>
+      <c r="M1008" s="3"/>
+      <c r="N1008" s="3"/>
+      <c r="O1008" s="3"/>
+      <c r="P1008" s="3"/>
+      <c r="Q1008" s="3"/>
+      <c r="R1008" s="3"/>
+      <c r="S1008" s="3"/>
+      <c r="T1008" s="3"/>
+      <c r="U1008" s="3"/>
+      <c r="V1008" s="3"/>
+      <c r="W1008" s="3"/>
+      <c r="X1008" s="3"/>
+      <c r="Y1008" s="3"/>
+      <c r="Z1008" s="3"/>
+      <c r="AA1008" s="3"/>
+    </row>
+    <row r="1009" ht="15.75" customHeight="1">
+      <c r="A1009" s="3"/>
+      <c r="B1009" s="3"/>
+      <c r="C1009" s="3"/>
+      <c r="D1009" s="3"/>
+      <c r="E1009" s="3"/>
+      <c r="F1009" s="3"/>
+      <c r="G1009" s="3"/>
+      <c r="H1009" s="3"/>
+      <c r="I1009" s="3"/>
+      <c r="J1009" s="3"/>
+      <c r="K1009" s="3"/>
+      <c r="L1009" s="3"/>
+      <c r="M1009" s="3"/>
+      <c r="N1009" s="3"/>
+      <c r="O1009" s="3"/>
+      <c r="P1009" s="3"/>
+      <c r="Q1009" s="3"/>
+      <c r="R1009" s="3"/>
+      <c r="S1009" s="3"/>
+      <c r="T1009" s="3"/>
+      <c r="U1009" s="3"/>
+      <c r="V1009" s="3"/>
+      <c r="W1009" s="3"/>
+      <c r="X1009" s="3"/>
+      <c r="Y1009" s="3"/>
+      <c r="Z1009" s="3"/>
+      <c r="AA1009" s="3"/>
+    </row>
+    <row r="1010" ht="15.75" customHeight="1">
+      <c r="A1010" s="3"/>
+      <c r="B1010" s="3"/>
+      <c r="C1010" s="3"/>
+      <c r="D1010" s="3"/>
+      <c r="E1010" s="3"/>
+      <c r="F1010" s="3"/>
+      <c r="G1010" s="3"/>
+      <c r="H1010" s="3"/>
+      <c r="I1010" s="3"/>
+      <c r="J1010" s="3"/>
+      <c r="K1010" s="3"/>
+      <c r="L1010" s="3"/>
+      <c r="M1010" s="3"/>
+      <c r="N1010" s="3"/>
+      <c r="O1010" s="3"/>
+      <c r="P1010" s="3"/>
+      <c r="Q1010" s="3"/>
+      <c r="R1010" s="3"/>
+      <c r="S1010" s="3"/>
+      <c r="T1010" s="3"/>
+      <c r="U1010" s="3"/>
+      <c r="V1010" s="3"/>
+      <c r="W1010" s="3"/>
+      <c r="X1010" s="3"/>
+      <c r="Y1010" s="3"/>
+      <c r="Z1010" s="3"/>
+      <c r="AA1010" s="3"/>
+    </row>
+    <row r="1011" ht="15.75" customHeight="1">
+      <c r="A1011" s="3"/>
+      <c r="B1011" s="3"/>
+      <c r="C1011" s="3"/>
+      <c r="D1011" s="3"/>
+      <c r="E1011" s="3"/>
+      <c r="F1011" s="3"/>
+      <c r="G1011" s="3"/>
+      <c r="H1011" s="3"/>
+      <c r="I1011" s="3"/>
+      <c r="J1011" s="3"/>
+      <c r="K1011" s="3"/>
+      <c r="L1011" s="3"/>
+      <c r="M1011" s="3"/>
+      <c r="N1011" s="3"/>
+      <c r="O1011" s="3"/>
+      <c r="P1011" s="3"/>
+      <c r="Q1011" s="3"/>
+      <c r="R1011" s="3"/>
+      <c r="S1011" s="3"/>
+      <c r="T1011" s="3"/>
+      <c r="U1011" s="3"/>
+      <c r="V1011" s="3"/>
+      <c r="W1011" s="3"/>
+      <c r="X1011" s="3"/>
+      <c r="Y1011" s="3"/>
+      <c r="Z1011" s="3"/>
+      <c r="AA1011" s="3"/>
+    </row>
+    <row r="1012" ht="15.75" customHeight="1">
+      <c r="A1012" s="3"/>
+      <c r="B1012" s="3"/>
+      <c r="C1012" s="3"/>
+      <c r="D1012" s="3"/>
+      <c r="E1012" s="3"/>
+      <c r="F1012" s="3"/>
+      <c r="G1012" s="3"/>
+      <c r="H1012" s="3"/>
+      <c r="I1012" s="3"/>
+      <c r="J1012" s="3"/>
+      <c r="K1012" s="3"/>
+      <c r="L1012" s="3"/>
+      <c r="M1012" s="3"/>
+      <c r="N1012" s="3"/>
+      <c r="O1012" s="3"/>
+      <c r="P1012" s="3"/>
+      <c r="Q1012" s="3"/>
+      <c r="R1012" s="3"/>
+      <c r="S1012" s="3"/>
+      <c r="T1012" s="3"/>
+      <c r="U1012" s="3"/>
+      <c r="V1012" s="3"/>
+      <c r="W1012" s="3"/>
+      <c r="X1012" s="3"/>
+      <c r="Y1012" s="3"/>
+      <c r="Z1012" s="3"/>
+      <c r="AA1012" s="3"/>
+    </row>
+    <row r="1013" ht="15.75" customHeight="1">
+      <c r="A1013" s="3"/>
+      <c r="B1013" s="3"/>
+      <c r="C1013" s="3"/>
+      <c r="D1013" s="3"/>
+      <c r="E1013" s="3"/>
+      <c r="F1013" s="3"/>
+      <c r="G1013" s="3"/>
+      <c r="H1013" s="3"/>
+      <c r="I1013" s="3"/>
+      <c r="J1013" s="3"/>
+      <c r="K1013" s="3"/>
+      <c r="L1013" s="3"/>
+      <c r="M1013" s="3"/>
+      <c r="N1013" s="3"/>
+      <c r="O1013" s="3"/>
+      <c r="P1013" s="3"/>
+      <c r="Q1013" s="3"/>
+      <c r="R1013" s="3"/>
+      <c r="S1013" s="3"/>
+      <c r="T1013" s="3"/>
+      <c r="U1013" s="3"/>
+      <c r="V1013" s="3"/>
+      <c r="W1013" s="3"/>
+      <c r="X1013" s="3"/>
+      <c r="Y1013" s="3"/>
+      <c r="Z1013" s="3"/>
+      <c r="AA1013" s="3"/>
+    </row>
+    <row r="1014" ht="15.75" customHeight="1">
+      <c r="A1014" s="3"/>
+      <c r="B1014" s="3"/>
+      <c r="C1014" s="3"/>
+      <c r="D1014" s="3"/>
+      <c r="E1014" s="3"/>
+      <c r="F1014" s="3"/>
+      <c r="G1014" s="3"/>
+      <c r="H1014" s="3"/>
+      <c r="I1014" s="3"/>
+      <c r="J1014" s="3"/>
+      <c r="K1014" s="3"/>
+      <c r="L1014" s="3"/>
+      <c r="M1014" s="3"/>
+      <c r="N1014" s="3"/>
+      <c r="O1014" s="3"/>
+      <c r="P1014" s="3"/>
+      <c r="Q1014" s="3"/>
+      <c r="R1014" s="3"/>
+      <c r="S1014" s="3"/>
+      <c r="T1014" s="3"/>
+      <c r="U1014" s="3"/>
+      <c r="V1014" s="3"/>
+      <c r="W1014" s="3"/>
+      <c r="X1014" s="3"/>
+      <c r="Y1014" s="3"/>
+      <c r="Z1014" s="3"/>
+      <c r="AA1014" s="3"/>
+    </row>
+    <row r="1015" ht="15.75" customHeight="1">
+      <c r="A1015" s="3"/>
+      <c r="B1015" s="3"/>
+      <c r="C1015" s="3"/>
+      <c r="D1015" s="3"/>
+      <c r="E1015" s="3"/>
+      <c r="F1015" s="3"/>
+      <c r="G1015" s="3"/>
+      <c r="H1015" s="3"/>
+      <c r="I1015" s="3"/>
+      <c r="J1015" s="3"/>
+      <c r="K1015" s="3"/>
+      <c r="L1015" s="3"/>
+      <c r="M1015" s="3"/>
+      <c r="N1015" s="3"/>
+      <c r="O1015" s="3"/>
+      <c r="P1015" s="3"/>
+      <c r="Q1015" s="3"/>
+      <c r="R1015" s="3"/>
+      <c r="S1015" s="3"/>
+      <c r="T1015" s="3"/>
+      <c r="U1015" s="3"/>
+      <c r="V1015" s="3"/>
+      <c r="W1015" s="3"/>
+      <c r="X1015" s="3"/>
+      <c r="Y1015" s="3"/>
+      <c r="Z1015" s="3"/>
+      <c r="AA1015" s="3"/>
+    </row>
+    <row r="1016" ht="15.75" customHeight="1">
+      <c r="A1016" s="3"/>
+      <c r="B1016" s="3"/>
+      <c r="C1016" s="3"/>
+      <c r="D1016" s="3"/>
+      <c r="E1016" s="3"/>
+      <c r="F1016" s="3"/>
+      <c r="G1016" s="3"/>
+      <c r="H1016" s="3"/>
+      <c r="I1016" s="3"/>
+      <c r="J1016" s="3"/>
+      <c r="K1016" s="3"/>
+      <c r="L1016" s="3"/>
+      <c r="M1016" s="3"/>
+      <c r="N1016" s="3"/>
+      <c r="O1016" s="3"/>
+      <c r="P1016" s="3"/>
+      <c r="Q1016" s="3"/>
+      <c r="R1016" s="3"/>
+      <c r="S1016" s="3"/>
+      <c r="T1016" s="3"/>
+      <c r="U1016" s="3"/>
+      <c r="V1016" s="3"/>
+      <c r="W1016" s="3"/>
+      <c r="X1016" s="3"/>
+      <c r="Y1016" s="3"/>
+      <c r="Z1016" s="3"/>
+      <c r="AA1016" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E7"/>
-    <hyperlink r:id="rId2" ref="H7"/>
-    <hyperlink r:id="rId3" ref="E8"/>
-    <hyperlink r:id="rId4" ref="H8"/>
-    <hyperlink r:id="rId5" ref="E9"/>
-    <hyperlink r:id="rId6" ref="H9"/>
-    <hyperlink r:id="rId7" ref="H10"/>
-    <hyperlink r:id="rId8" ref="H11"/>
-    <hyperlink r:id="rId9" ref="E12"/>
-    <hyperlink r:id="rId10" ref="H12"/>
-    <hyperlink r:id="rId11" ref="E13"/>
-    <hyperlink r:id="rId12" ref="H13"/>
-    <hyperlink r:id="rId13" ref="E14"/>
-    <hyperlink r:id="rId14" ref="H14"/>
-    <hyperlink r:id="rId15" ref="H15"/>
-    <hyperlink r:id="rId16" ref="H16"/>
-    <hyperlink r:id="rId17" ref="H17"/>
-    <hyperlink r:id="rId18" ref="H18"/>
-    <hyperlink r:id="rId19" ref="H19"/>
-    <hyperlink r:id="rId20" ref="H20"/>
-    <hyperlink r:id="rId21" ref="H21"/>
-    <hyperlink r:id="rId22" ref="H22"/>
-    <hyperlink r:id="rId23" ref="H23"/>
-    <hyperlink r:id="rId24" ref="H24"/>
-    <hyperlink r:id="rId25" ref="H25"/>
-    <hyperlink r:id="rId26" ref="H26"/>
-    <hyperlink r:id="rId27" ref="H27"/>
-    <hyperlink r:id="rId28" ref="H28"/>
+    <hyperlink r:id="rId2" ref="E7"/>
+    <hyperlink r:id="rId3" ref="H7"/>
+    <hyperlink r:id="rId4" ref="E8"/>
+    <hyperlink r:id="rId5" ref="H8"/>
+    <hyperlink r:id="rId6" ref="E9"/>
+    <hyperlink r:id="rId7" ref="H9"/>
+    <hyperlink r:id="rId8" ref="H10"/>
+    <hyperlink r:id="rId9" ref="H11"/>
+    <hyperlink r:id="rId10" ref="E12"/>
+    <hyperlink r:id="rId11" ref="H12"/>
+    <hyperlink r:id="rId12" ref="E13"/>
+    <hyperlink r:id="rId13" ref="H13"/>
+    <hyperlink r:id="rId14" ref="E14"/>
+    <hyperlink r:id="rId15" ref="H14"/>
+    <hyperlink r:id="rId16" ref="H15"/>
+    <hyperlink r:id="rId17" ref="H16"/>
+    <hyperlink r:id="rId18" ref="H17"/>
+    <hyperlink r:id="rId19" ref="H18"/>
+    <hyperlink r:id="rId20" ref="H19"/>
+    <hyperlink r:id="rId21" ref="H20"/>
+    <hyperlink r:id="rId22" ref="H21"/>
+    <hyperlink r:id="rId23" ref="H22"/>
+    <hyperlink r:id="rId24" ref="H23"/>
+    <hyperlink r:id="rId25" ref="H24"/>
+    <hyperlink r:id="rId26" ref="H25"/>
+    <hyperlink r:id="rId27" ref="H26"/>
+    <hyperlink r:id="rId28" ref="H27"/>
     <hyperlink r:id="rId29" ref="H29"/>
     <hyperlink r:id="rId30" ref="H30"/>
     <hyperlink r:id="rId31" ref="H31"/>
+    <hyperlink r:id="rId32" ref="H32"/>
+    <hyperlink r:id="rId33" ref="H33"/>
+    <hyperlink r:id="rId34" ref="H34"/>
+    <hyperlink r:id="rId35" ref="H35"/>
+    <hyperlink r:id="rId36" ref="H36"/>
+    <hyperlink r:id="rId37" ref="H37"/>
+    <hyperlink r:id="rId38" ref="H38"/>
+    <hyperlink r:id="rId39" ref="H39"/>
+    <hyperlink r:id="rId40" ref="H40"/>
+    <hyperlink r:id="rId41" ref="H41"/>
+    <hyperlink r:id="rId42" ref="H42"/>
+    <hyperlink r:id="rId43" ref="H43"/>
+    <hyperlink r:id="rId44" ref="H44"/>
+    <hyperlink r:id="rId45" ref="H45"/>
+    <hyperlink r:id="rId46" ref="H46"/>
+    <hyperlink r:id="rId47" ref="H47"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.66666666666667" footer="0.0" header="0.0" left="1.0" right="1.0" top="1.66666666666667"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId32"/>
+  <drawing r:id="rId48"/>
+  <legacyDrawing r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>